<commit_message>
solution ready for 1 device
</commit_message>
<xml_diff>
--- a/devices/edge_devices_v0.0.1.xlsx
+++ b/devices/edge_devices_v0.0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044bsj\Desktop\API_app_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA242136-184F-4E27-9E92-FA4DBD1C00BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399D9E8C-BA94-485C-B2E9-9E08F84CBF6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
   </bookViews>
   <sheets>
     <sheet name="DEVICE_CONFIG" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>DEVICE TYPE ID</t>
   </si>
@@ -65,9 +65,6 @@
     <t>pavel.halama@siemens.com</t>
   </si>
   <si>
-    <t>device_new</t>
-  </si>
-  <si>
     <t>IP ADRESS*</t>
   </si>
   <si>
@@ -182,10 +179,10 @@
     <t>SECONDARY DNS IP*</t>
   </si>
   <si>
-    <t>true, true</t>
-  </si>
-  <si>
-    <t>192.168.1.1, 192.168.1.2</t>
+    <t>true, false</t>
+  </si>
+  <si>
+    <t>new22</t>
   </si>
 </sst>
 </file>
@@ -567,8 +564,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -605,10 +602,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -622,8 +619,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,43 +650,43 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="L1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -697,49 +694,60 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -785,12 +793,9 @@
       <c r="E17" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E17" xr:uid="{A18734B2-F05C-4437-A90F-A60D2A75CCEB}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E17" xr:uid="{A18734B2-F05C-4437-A90F-A60D2A75CCEB}">
       <formula1>"enabled, disabled"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{2DEADC07-63FF-4EDA-B96E-A313F85EA7A2}">
-      <formula1>"true, false"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -820,13 +825,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -834,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -869,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -877,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -906,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -940,22 +945,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -963,16 +968,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished reading excel file and creating onboarding file
</commit_message>
<xml_diff>
--- a/devices/edge_devices_v0.0.1.xlsx
+++ b/devices/edge_devices_v0.0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044bsj\Desktop\API_app_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E93AAE-A77B-48E7-94D6-4716D7A659DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2B17C5-BB17-4F4F-8766-EA5AA24126F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
   </bookViews>
   <sheets>
     <sheet name="DEVICE_CONFIG" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>DEVICE TYPE ID</t>
   </si>
@@ -74,9 +74,6 @@
     <t>RANGE</t>
   </si>
   <si>
-    <t xml:space="preserve">DOCKER IP </t>
-  </si>
-  <si>
     <t>NTP SERVER</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>192.168.1.8</t>
   </si>
   <si>
-    <t>172.16.0.0/16</t>
-  </si>
-  <si>
     <t>192.168.80.144:3128</t>
   </si>
   <si>
@@ -173,13 +167,22 @@
     <t>true, false</t>
   </si>
   <si>
-    <t>new22</t>
-  </si>
-  <si>
     <t>L2 ACESS*</t>
   </si>
   <si>
     <t>NETWORK MASK</t>
+  </si>
+  <si>
+    <t>DOCKER IP</t>
+  </si>
+  <si>
+    <t>new25</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,12 +217,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -233,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -243,7 +240,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +558,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,10 +595,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -616,8 +612,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,37 +649,37 @@
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="L1" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -691,43 +687,43 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -805,8 +801,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -836,10 +832,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -857,7 +853,7 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -871,15 +867,12 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -891,24 +884,29 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF52AFF8-10A9-47DF-B863-80E6A4CE4562}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>11</v>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -922,8 +920,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,22 +940,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -965,19 +963,30 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0EF77AEC-E69A-4071-8C4A-A16613E4BBF1}">
+      <formula1>"http, https"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
application ready for 1 device
</commit_message>
<xml_diff>
--- a/devices/edge_devices_v0.0.1.xlsx
+++ b/devices/edge_devices_v0.0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044bsj\Desktop\API_app_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2B17C5-BB17-4F4F-8766-EA5AA24126F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3406394-9F61-4B9D-8382-D2910DFF6C4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
   </bookViews>
   <sheets>
     <sheet name="DEVICE_CONFIG" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>DEVICE TYPE ID</t>
   </si>
@@ -128,33 +128,15 @@
     <t>255.255.255.0</t>
   </si>
   <si>
-    <t>192.168.1.1</t>
-  </si>
-  <si>
-    <t>8.8.8.8</t>
-  </si>
-  <si>
     <t>192.168.1.8</t>
   </si>
   <si>
-    <t>192.168.80.144:3128</t>
-  </si>
-  <si>
     <t>http</t>
   </si>
   <si>
-    <t>192.168.1.107</t>
-  </si>
-  <si>
-    <t>1234, 5678</t>
-  </si>
-  <si>
     <t xml:space="preserve">true, false </t>
   </si>
   <si>
-    <t xml:space="preserve">disabled, enabled </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 00:0C:29:FC:EA:3E, 00:0C:29:FC:EA:48</t>
   </si>
   <si>
@@ -164,9 +146,6 @@
     <t>SECONDARY DNS IP*</t>
   </si>
   <si>
-    <t>true, false</t>
-  </si>
-  <si>
     <t>L2 ACESS*</t>
   </si>
   <si>
@@ -176,13 +155,31 @@
     <t>DOCKER IP</t>
   </si>
   <si>
-    <t>new25</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
+    <t>device1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false, false </t>
+  </si>
+  <si>
+    <t>false,false</t>
+  </si>
+  <si>
+    <t>disabled, disabled</t>
+  </si>
+  <si>
+    <t>255.255.255.0, 255.255.255.0</t>
+  </si>
+  <si>
+    <t>192.168.1.1, 192.168.1.1</t>
+  </si>
+  <si>
+    <t>192.168.1.108, 192.168.1.106</t>
+  </si>
+  <si>
+    <t>false, true</t>
+  </si>
+  <si>
+    <t>0.pool.time.org</t>
   </si>
 </sst>
 </file>
@@ -558,7 +555,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,7 +595,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -612,8 +609,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,9 +621,9 @@
     <col min="4" max="4" width="40.6640625" customWidth="1"/>
     <col min="5" max="5" width="28.44140625" customWidth="1"/>
     <col min="6" max="6" width="25.21875" customWidth="1"/>
-    <col min="7" max="7" width="22.109375" customWidth="1"/>
-    <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
     <col min="11" max="11" width="26.44140625" customWidth="1"/>
     <col min="12" max="12" width="26" customWidth="1"/>
@@ -673,13 +670,13 @@
         <v>24</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -693,37 +690,33 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -821,7 +814,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -832,7 +825,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -853,7 +846,7 @@
   <dimension ref="A2:B3"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -886,8 +879,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,6 +900,9 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -920,7 +916,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -962,23 +958,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draft application ready for onboarding multiple devices
</commit_message>
<xml_diff>
--- a/devices/edge_devices_v0.0.1.xlsx
+++ b/devices/edge_devices_v0.0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044bsj\Desktop\API_app_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3406394-9F61-4B9D-8382-D2910DFF6C4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9769748-DDB7-470B-96D9-7FB4ED4E1A69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6C038622-31ED-4E4C-8AD3-BA89D21E8C25}"/>
   </bookViews>
   <sheets>
     <sheet name="DEVICE_CONFIG" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>DEVICE TYPE ID</t>
   </si>
@@ -137,9 +137,6 @@
     <t xml:space="preserve">true, false </t>
   </si>
   <si>
-    <t xml:space="preserve"> 00:0C:29:FC:EA:3E, 00:0C:29:FC:EA:48</t>
-  </si>
-  <si>
     <t>PRIMARY DNS IP*</t>
   </si>
   <si>
@@ -179,17 +176,50 @@
     <t>false, true</t>
   </si>
   <si>
-    <t>0.pool.time.org</t>
+    <t>device2</t>
+  </si>
+  <si>
+    <t>0.pool.ntp.org</t>
+  </si>
+  <si>
+    <t>192.168.1.95</t>
+  </si>
+  <si>
+    <t>00:0C:29:EA:B9:21</t>
+  </si>
+  <si>
+    <t>00:0C:29:FC:EA:3E, 00:0C:29:FC:EA:48</t>
+  </si>
+  <si>
+    <t>disabled</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false </t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>0.pool.ntp.org, time.google.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -552,10 +582,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C751101-BB4C-4C9A-B06B-559B9CBC5A46}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +625,21 @@
         <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -609,8 +653,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,13 +714,13 @@
         <v>24</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -690,50 +734,76 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="N3" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -779,6 +849,7 @@
       <c r="E17" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E17" xr:uid="{A18734B2-F05C-4437-A90F-A60D2A75CCEB}">
       <formula1>"enabled, disabled"</formula1>
@@ -792,10 +863,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43BAD28-0446-43ED-BF03-FF5BB616F954}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -814,7 +885,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
@@ -834,7 +905,22 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -843,10 +929,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C3053-0E68-46E8-ADDA-BCB9E625C1F9}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -860,12 +946,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -877,10 +968,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF52AFF8-10A9-47DF-B863-80E6A4CE4562}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,6 +996,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -914,10 +1013,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2DF393E-C283-449B-98D8-D3E6077E93EA}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -962,9 +1061,17 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{0EF77AEC-E69A-4071-8C4A-A16613E4BBF1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{0EF77AEC-E69A-4071-8C4A-A16613E4BBF1}">
       <formula1>"http, https"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>